<commit_message>
Turkish+ Nippon RPA finished
</commit_message>
<xml_diff>
--- a/TurkishCargo/Test.xlsx
+++ b/TurkishCargo/Test.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>WONumber</t>
   </si>
@@ -32,64 +32,64 @@
     <t>ReferenceNumber</t>
   </si>
   <si>
-    <t>235-34474882</t>
-  </si>
-  <si>
-    <t>22E0007436</t>
-  </si>
-  <si>
-    <t>235-37989943</t>
-  </si>
-  <si>
-    <t>235-38048894</t>
-  </si>
-  <si>
-    <t>DJYYZA4071377</t>
-  </si>
-  <si>
-    <t>DJYYZA4071372</t>
-  </si>
-  <si>
-    <t>DJYYZA4071368</t>
-  </si>
-  <si>
-    <t>235-33206526</t>
-  </si>
-  <si>
-    <t>DJANKA4070970</t>
-  </si>
-  <si>
-    <t>23K0232316</t>
-  </si>
-  <si>
-    <t>235-37083992</t>
-  </si>
-  <si>
-    <t>235-38196572</t>
-  </si>
-  <si>
-    <t>DJAMSA4070103</t>
-  </si>
-  <si>
-    <t>235-36599920</t>
-  </si>
-  <si>
-    <t>DJBOMA4069910</t>
-  </si>
-  <si>
-    <t>22C0420766</t>
-  </si>
-  <si>
-    <t>235-36640866</t>
-  </si>
-  <si>
-    <t>DJANKA4069375</t>
-  </si>
-  <si>
-    <t>23K0232001</t>
-  </si>
-  <si>
     <t>Waybill Number</t>
+  </si>
+  <si>
+    <t>235-36155346</t>
+  </si>
+  <si>
+    <t>DJSJUA4241863</t>
+  </si>
+  <si>
+    <t>235-36298102</t>
+  </si>
+  <si>
+    <t>DJCVGA4241735</t>
+  </si>
+  <si>
+    <t>235-36298065</t>
+  </si>
+  <si>
+    <t>DJCVGA4241725</t>
+  </si>
+  <si>
+    <t>235-36297586</t>
+  </si>
+  <si>
+    <t>DJJNBA4241335</t>
+  </si>
+  <si>
+    <t>235-36155162</t>
+  </si>
+  <si>
+    <t>DJSAVA4241086</t>
+  </si>
+  <si>
+    <t>DJDURA4240721</t>
+  </si>
+  <si>
+    <t>235-33973601</t>
+  </si>
+  <si>
+    <t>DJAMSA4239118</t>
+  </si>
+  <si>
+    <t>235-36297726</t>
+  </si>
+  <si>
+    <t>DJSTRA4238475</t>
+  </si>
+  <si>
+    <t>235-39888052</t>
+  </si>
+  <si>
+    <t>DJSINA4238206</t>
+  </si>
+  <si>
+    <t>235-36925383</t>
+  </si>
+  <si>
+    <t>DJISTA4238100</t>
   </si>
 </sst>
 </file>
@@ -411,7 +411,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="A2" sqref="A2:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -423,7 +423,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -434,57 +434,57 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="C2" s="1">
+        <v>2340126729</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3">
-        <v>2460116877</v>
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
       </c>
       <c r="C3">
-        <v>2460116877</v>
+        <v>2200250137</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C4">
-        <v>2101099088</v>
+        <v>2200250134</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C5">
-        <v>2101099087</v>
+        <v>2780468943</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C6">
-        <v>2101099086</v>
+        <v>2330055233</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -492,54 +492,54 @@
         <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" t="s">
-        <v>11</v>
+        <v>13</v>
+      </c>
+      <c r="C7">
+        <v>2790022451</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8">
-        <v>2711768766</v>
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
       </c>
       <c r="C8">
-        <v>2711768766</v>
+        <v>2482459020</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C9">
-        <v>2482440833</v>
+        <v>2570304342</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" t="s">
-        <v>17</v>
+        <v>19</v>
+      </c>
+      <c r="C10">
+        <v>2711779354</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" t="s">
-        <v>20</v>
+        <v>21</v>
+      </c>
+      <c r="C11">
+        <v>2640264509</v>
       </c>
     </row>
   </sheetData>

</xml_diff>